<commit_message>
Updated final BOM. Final 'd' version of gerbers, which got sent to JLCPCB.
</commit_message>
<xml_diff>
--- a/RCM-Comm_v4/RCM-Comm_v4_BOM.xlsx
+++ b/RCM-Comm_v4/RCM-Comm_v4_BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABCF2EF-A776-4BBF-91B1-9199DDF18B70}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D31D9A-63A8-42F2-9242-96E6B739BCC0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
   <si>
     <t>Mfg Part #</t>
   </si>
@@ -146,15 +146,6 @@
     <t>SWITCH TACTILE SPST-NO 0.02A 15V</t>
   </si>
   <si>
-    <t>Spacer</t>
-  </si>
-  <si>
-    <t>Nut</t>
-  </si>
-  <si>
-    <t>Bolt</t>
-  </si>
-  <si>
     <t>XPC240300S-02</t>
   </si>
   <si>
@@ -162,6 +153,51 @@
   </si>
   <si>
     <t>XPC240300S-02-ND</t>
+  </si>
+  <si>
+    <t>91772A058</t>
+  </si>
+  <si>
+    <t>McMaseter-Carr</t>
+  </si>
+  <si>
+    <t>Passivated 18-8 Stainless Steel Pan Head Phillips Screw, 0-80 Thread, 7/32" Long</t>
+  </si>
+  <si>
+    <t>91841A115</t>
+  </si>
+  <si>
+    <t>18-8 Stainless Steel Hex Nut, 0-80 Thread Size</t>
+  </si>
+  <si>
+    <t>18-8 Stainless Steel Unthreaded Spacer, 1/8" OD, 1/8" Long, for Number 0 Screw Size</t>
+  </si>
+  <si>
+    <t>92321A005</t>
+  </si>
+  <si>
+    <t>Samtec</t>
+  </si>
+  <si>
+    <t>SSQ-116-03-G-D</t>
+  </si>
+  <si>
+    <t>2 x 16 .1" female header with long pins</t>
+  </si>
+  <si>
+    <t>C6, C7</t>
+  </si>
+  <si>
+    <t>1276-6455-1-ND</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics</t>
+  </si>
+  <si>
+    <t>CL21A106KOQNNNG</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 16V X5R 0805</t>
   </si>
 </sst>
 </file>
@@ -210,8 +246,8 @@
       <family val="2"/>
     </font>
     <font>
+      <u/>
       <sz val="10"/>
-      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -249,7 +285,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -328,21 +364,42 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -762,7 +819,7 @@
   <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -780,17 +837,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C2" s="13"/>
@@ -798,6 +855,7 @@
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
+      <c r="H2" s="31"/>
       <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -828,11 +886,11 @@
         <v>2</v>
       </c>
       <c r="H4" s="18"/>
-      <c r="I4" s="29"/>
+      <c r="I4" s="32"/>
       <c r="J4" s="26"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="17">
+      <c r="A5" s="30">
         <v>1</v>
       </c>
       <c r="B5" s="15">
@@ -854,11 +912,11 @@
         <v>22</v>
       </c>
       <c r="H5" s="18"/>
-      <c r="I5" s="29"/>
+      <c r="I5" s="32"/>
       <c r="J5" s="26"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="17">
+      <c r="A6" s="30">
         <v>2</v>
       </c>
       <c r="B6" s="15">
@@ -867,16 +925,24 @@
       <c r="C6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="D6" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="H6" s="18"/>
-      <c r="I6" s="29"/>
+      <c r="I6" s="32"/>
       <c r="J6" s="26"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="17">
+      <c r="A7" s="30">
         <v>3</v>
       </c>
       <c r="B7" s="15">
@@ -885,7 +951,7 @@
       <c r="C7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="34" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -898,11 +964,11 @@
         <v>25</v>
       </c>
       <c r="H7" s="18"/>
-      <c r="I7" s="29"/>
+      <c r="I7" s="32"/>
       <c r="J7" s="26"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="17">
+      <c r="A8" s="30">
         <v>4</v>
       </c>
       <c r="B8" s="15">
@@ -911,7 +977,7 @@
       <c r="C8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="34" t="s">
         <v>27</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -924,11 +990,11 @@
         <v>29</v>
       </c>
       <c r="H8" s="18"/>
-      <c r="I8" s="29"/>
+      <c r="I8" s="32"/>
       <c r="J8" s="26"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="17">
+      <c r="A9" s="30">
         <v>5</v>
       </c>
       <c r="B9" s="15">
@@ -937,7 +1003,7 @@
       <c r="C9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="34" t="s">
         <v>27</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -950,11 +1016,11 @@
         <v>32</v>
       </c>
       <c r="H9" s="18"/>
-      <c r="I9" s="29"/>
+      <c r="I9" s="32"/>
       <c r="J9" s="26"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="10">
+      <c r="A10" s="32">
         <v>6</v>
       </c>
       <c r="B10" s="15">
@@ -963,7 +1029,7 @@
       <c r="C10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="35" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="4">
@@ -976,10 +1042,10 @@
         <v>35</v>
       </c>
       <c r="H10" s="9"/>
-      <c r="I10" s="10"/>
+      <c r="I10" s="32"/>
     </row>
     <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="17">
+      <c r="A11" s="30">
         <v>7</v>
       </c>
       <c r="B11" s="15">
@@ -988,7 +1054,7 @@
       <c r="C11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="35" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="4" t="s">
@@ -1001,10 +1067,10 @@
         <v>38</v>
       </c>
       <c r="H11" s="21"/>
-      <c r="I11" s="10"/>
+      <c r="I11" s="32"/>
     </row>
     <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="17">
+      <c r="A12" s="30">
         <v>8</v>
       </c>
       <c r="B12" s="15">
@@ -1013,7 +1079,7 @@
       <c r="C12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="35" t="s">
         <v>40</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -1026,102 +1092,135 @@
         <v>42</v>
       </c>
       <c r="H12" s="21"/>
-      <c r="I12" s="10"/>
+      <c r="I12" s="32"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="17">
+      <c r="A13" s="30">
         <v>9</v>
       </c>
       <c r="B13" s="15">
         <v>1</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I13" s="10"/>
+      <c r="D13" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="31"/>
+      <c r="I13" s="32"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="17">
+      <c r="A14" s="30">
         <v>10</v>
       </c>
       <c r="B14" s="15">
         <v>1</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2" t="s">
-        <v>43</v>
+      <c r="C14" s="40"/>
+      <c r="D14" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>51</v>
       </c>
       <c r="H14" s="21"/>
-      <c r="I14" s="10"/>
+      <c r="I14" s="32"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="17">
+      <c r="A15" s="30">
         <v>11</v>
       </c>
       <c r="B15" s="15">
         <v>1</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2" t="s">
-        <v>44</v>
+      <c r="C15" s="40"/>
+      <c r="D15" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>50</v>
       </c>
       <c r="H15" s="21"/>
-      <c r="I15" s="10"/>
+      <c r="I15" s="32"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="17">
+      <c r="A16" s="30">
         <v>12</v>
       </c>
       <c r="B16" s="15">
         <v>1</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2" t="s">
-        <v>45</v>
+      <c r="C16" s="40"/>
+      <c r="D16" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>48</v>
       </c>
       <c r="H16" s="21"/>
-      <c r="I16" s="10"/>
+      <c r="I16" s="32"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="17"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
+      <c r="A17" s="30">
+        <v>13</v>
+      </c>
+      <c r="B17" s="15">
+        <v>2</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="40" t="s">
+        <v>60</v>
+      </c>
       <c r="H17" s="18"/>
-      <c r="I17" s="10"/>
+      <c r="I17" s="32"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
       <c r="B18" s="15"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
       <c r="H18" s="21"/>
       <c r="I18" s="10"/>
     </row>
@@ -1372,7 +1471,7 @@
       <c r="E41" s="4"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
-      <c r="H41" s="34"/>
+      <c r="H41" s="33"/>
       <c r="I41" s="29"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -1393,8 +1492,8 @@
       <c r="E43" s="14"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="G45" s="32"/>
-      <c r="H45" s="32"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
       <c r="I45" s="26"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -1427,8 +1526,8 @@
       <c r="C52" s="26"/>
       <c r="D52" s="26"/>
       <c r="E52" s="26"/>
-      <c r="F52" s="33"/>
-      <c r="G52" s="33"/>
+      <c r="F52" s="39"/>
+      <c r="G52" s="39"/>
       <c r="I52" s="27"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
@@ -1437,8 +1536,8 @@
       <c r="C53" s="26"/>
       <c r="D53" s="26"/>
       <c r="E53" s="26"/>
-      <c r="F53" s="33"/>
-      <c r="G53" s="33"/>
+      <c r="F53" s="39"/>
+      <c r="G53" s="39"/>
       <c r="I53" s="27"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
@@ -1447,8 +1546,8 @@
       <c r="C54" s="26"/>
       <c r="D54" s="26"/>
       <c r="E54" s="26"/>
-      <c r="F54" s="30"/>
-      <c r="G54" s="30"/>
+      <c r="F54" s="36"/>
+      <c r="G54" s="36"/>
       <c r="I54" s="28"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
@@ -1468,8 +1567,16 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="E16" r:id="rId1" display="https://www.mcmaster.com/91772A058" xr:uid="{AAF77D57-062C-4717-97B2-96DBE352283B}"/>
+    <hyperlink ref="F16" r:id="rId2" display="https://www.mcmaster.com/91772A058" xr:uid="{6A8270A4-4FFF-436D-B7AA-3F9193EF115A}"/>
+    <hyperlink ref="F15" r:id="rId3" display="https://www.mcmaster.com/91841A115" xr:uid="{BF108449-030E-4E62-990F-FC4ACDB22089}"/>
+    <hyperlink ref="E15" r:id="rId4" display="https://www.mcmaster.com/91841A115" xr:uid="{8448E8C7-1025-4236-818C-C84442B60A6B}"/>
+    <hyperlink ref="F14" r:id="rId5" tooltip="Close" display="https://www.mcmaster.com/92321A005" xr:uid="{6A949477-07BA-47D0-8EFA-1A6573B0FC4C}"/>
+    <hyperlink ref="E14" r:id="rId6" tooltip="Close" display="https://www.mcmaster.com/92321A005" xr:uid="{E7622FF5-A06E-449B-87F1-917D64E78445}"/>
+  </hyperlinks>
   <pageMargins left="0.22" right="0.28999999999999998" top="0.3" bottom="0.4" header="0.22" footer="0.28999999999999998"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId7"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>